<commit_message>
fixed error in dataset - bad b_Vcmax values
</commit_message>
<xml_diff>
--- a/Growth_chamber_dataset.xlsx
+++ b/Growth_chamber_dataset.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Research/Thesis/Growth chamber/Summer 2013/Writing/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D69231-688E-8743-9047-A6170A77D905}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="6500" yWindow="5020" windowWidth="27760" windowHeight="16380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final_data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -480,7 +481,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -578,6 +579,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -845,11 +849,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BY364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
-      <selection activeCell="BV2" sqref="BV2"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BW14" sqref="BW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,7 +1267,7 @@
         <v>-2.4009655670000001</v>
       </c>
       <c r="BG2" s="3">
-        <v>9000</v>
+        <v>0.39398183599999997</v>
       </c>
       <c r="BH2" s="3">
         <v>-6.8617010000000004E-3</v>
@@ -1496,7 +1500,7 @@
         <v>-1.858295534</v>
       </c>
       <c r="BG3" s="3">
-        <v>9000</v>
+        <v>0.30932826299999999</v>
       </c>
       <c r="BH3" s="3">
         <v>-4.9553970000000003E-3</v>
@@ -1729,7 +1733,7 @@
         <v>0.72270254199999995</v>
       </c>
       <c r="BG4" s="3">
-        <v>9000</v>
+        <v>0.18575140300000001</v>
       </c>
       <c r="BH4" s="3">
         <v>-2.7576179999999999E-3</v>
@@ -1962,7 +1966,7 @@
         <v>-0.38634216100000002</v>
       </c>
       <c r="BG5" s="3">
-        <v>9000</v>
+        <v>0.18418361699999999</v>
       </c>
       <c r="BH5" s="3">
         <v>-2.074116E-3</v>
@@ -2428,7 +2432,7 @@
         <v>-1.238408701</v>
       </c>
       <c r="BG7" s="3">
-        <v>9000</v>
+        <v>0.12299028200000001</v>
       </c>
       <c r="BH7" s="3">
         <v>-7.5381999999999999E-4</v>
@@ -2661,7 +2665,7 @@
         <v>0.88978135800000002</v>
       </c>
       <c r="BG8" s="3">
-        <v>9000</v>
+        <v>6.3512178000000002E-2</v>
       </c>
       <c r="BH8" s="3">
         <v>-2.04594E-4</v>
@@ -2894,7 +2898,7 @@
         <v>0.84275978600000001</v>
       </c>
       <c r="BG9" s="3">
-        <v>9000</v>
+        <v>9.7909051999999996E-2</v>
       </c>
       <c r="BH9" s="3">
         <v>-8.1868499999999999E-4</v>
@@ -3127,7 +3131,7 @@
         <v>1.1332395580000001</v>
       </c>
       <c r="BG10" s="3">
-        <v>9000</v>
+        <v>0.14248280599999999</v>
       </c>
       <c r="BH10" s="3">
         <v>-2.2965820000000001E-3</v>
@@ -3360,7 +3364,7 @@
         <v>2.2336579109999999</v>
       </c>
       <c r="BG11" s="3">
-        <v>9000</v>
+        <v>4.4867701000000003E-2</v>
       </c>
       <c r="BH11" s="3">
         <v>-7.0517699999999997E-4</v>
@@ -3593,7 +3597,7 @@
         <v>0.50814128800000002</v>
       </c>
       <c r="BG12" s="3">
-        <v>9000</v>
+        <v>0.18645382699999999</v>
       </c>
       <c r="BH12" s="3">
         <v>-3.230821E-3</v>
@@ -3826,7 +3830,7 @@
         <v>0.94080662299999995</v>
       </c>
       <c r="BG13" s="3">
-        <v>9000</v>
+        <v>0.14581482700000001</v>
       </c>
       <c r="BH13" s="3">
         <v>-2.2158690000000001E-3</v>
@@ -4059,7 +4063,7 @@
         <v>1.8646302699999999</v>
       </c>
       <c r="BG14" s="3">
-        <v>9000</v>
+        <v>6.1068588E-2</v>
       </c>
       <c r="BH14" s="3">
         <v>-8.1070600000000001E-4</v>
@@ -4292,7 +4296,7 @@
         <v>2.0159385599999999</v>
       </c>
       <c r="BG15" s="3">
-        <v>9000</v>
+        <v>8.4369176000000004E-2</v>
       </c>
       <c r="BH15" s="3">
         <v>-1.4840599999999999E-3</v>
@@ -4525,7 +4529,7 @@
         <v>1.144634522</v>
       </c>
       <c r="BG16" s="3">
-        <v>9000</v>
+        <v>0.11638238200000001</v>
       </c>
       <c r="BH16" s="3">
         <v>-1.8356939999999999E-3</v>
@@ -4758,7 +4762,7 @@
         <v>1.860322746</v>
       </c>
       <c r="BG17" s="3">
-        <v>9000</v>
+        <v>6.6831248999999995E-2</v>
       </c>
       <c r="BH17" s="3">
         <v>-8.8902399999999998E-4</v>
@@ -4991,7 +4995,7 @@
         <v>-9.3275643000000005E-2</v>
       </c>
       <c r="BG18" s="3">
-        <v>9000</v>
+        <v>0.20389483999999999</v>
       </c>
       <c r="BH18" s="3">
         <v>-3.0725769999999999E-3</v>
@@ -5224,7 +5228,7 @@
         <v>-0.61031195500000002</v>
       </c>
       <c r="BG19" s="3">
-        <v>9000</v>
+        <v>0.29066015699999997</v>
       </c>
       <c r="BH19" s="3">
         <v>-4.5630219999999999E-3</v>
@@ -5457,7 +5461,7 @@
         <v>-0.57087256799999997</v>
       </c>
       <c r="BG20" s="3">
-        <v>9000</v>
+        <v>0.28854874699999999</v>
       </c>
       <c r="BH20" s="3">
         <v>-4.171831E-3</v>
@@ -5690,7 +5694,7 @@
         <v>-3.8079573999999998E-2</v>
       </c>
       <c r="BG21" s="3">
-        <v>9000</v>
+        <v>0.205808407</v>
       </c>
       <c r="BH21" s="3">
         <v>-3.345378E-3</v>
@@ -5923,7 +5927,7 @@
         <v>-1.3134393440000001</v>
       </c>
       <c r="BG22" s="3">
-        <v>9000</v>
+        <v>0.35242388499999999</v>
       </c>
       <c r="BH22" s="3">
         <v>-5.6057169999999996E-3</v>
@@ -6156,7 +6160,7 @@
         <v>-0.40957481099999998</v>
       </c>
       <c r="BG23" s="3">
-        <v>9000</v>
+        <v>0.26646164700000002</v>
       </c>
       <c r="BH23" s="3">
         <v>-3.7564970000000001E-3</v>
@@ -6389,7 +6393,7 @@
         <v>-0.34454659199999998</v>
       </c>
       <c r="BG24" s="3">
-        <v>9000</v>
+        <v>0.263503551</v>
       </c>
       <c r="BH24" s="3">
         <v>-3.9297539999999997E-3</v>
@@ -6855,7 +6859,7 @@
         <v>-6.5825117000000002E-2</v>
       </c>
       <c r="BG26" s="3">
-        <v>9000</v>
+        <v>0.21641431999999999</v>
       </c>
       <c r="BH26" s="3">
         <v>-2.6124130000000001E-3</v>
@@ -7088,7 +7092,7 @@
         <v>-0.81257440800000003</v>
       </c>
       <c r="BG27" s="3">
-        <v>9000</v>
+        <v>0.24195156500000001</v>
       </c>
       <c r="BH27" s="3">
         <v>-3.7492250000000001E-3</v>
@@ -7321,7 +7325,7 @@
         <v>-0.60926670299999997</v>
       </c>
       <c r="BG28" s="3">
-        <v>9000</v>
+        <v>0.24891769399999999</v>
       </c>
       <c r="BH28" s="3">
         <v>-3.744439E-3</v>
@@ -7554,7 +7558,7 @@
         <v>3.6681469000000001E-2</v>
       </c>
       <c r="BG29" s="3">
-        <v>9000</v>
+        <v>0.22537722499999999</v>
       </c>
       <c r="BH29" s="3">
         <v>-3.322813E-3</v>
@@ -7787,7 +7791,7 @@
         <v>0.18718072199999999</v>
       </c>
       <c r="BG30" s="3">
-        <v>9000</v>
+        <v>0.19161222999999999</v>
       </c>
       <c r="BH30" s="3">
         <v>-2.1247900000000001E-3</v>
@@ -8020,7 +8024,7 @@
         <v>-0.23530422300000001</v>
       </c>
       <c r="BG31" s="3">
-        <v>9000</v>
+        <v>0.23438695900000001</v>
       </c>
       <c r="BH31" s="3">
         <v>-2.8958289999999999E-3</v>
@@ -8253,7 +8257,7 @@
         <v>-7.2888125999999998E-2</v>
       </c>
       <c r="BG32" s="3">
-        <v>9000</v>
+        <v>0.19726584799999999</v>
       </c>
       <c r="BH32" s="3">
         <v>-2.2168259999999999E-3</v>
@@ -8486,7 +8490,7 @@
         <v>1.3389205E-2</v>
       </c>
       <c r="BG33" s="3">
-        <v>9000</v>
+        <v>0.211677963</v>
       </c>
       <c r="BH33" s="3">
         <v>-2.3392539999999998E-3</v>
@@ -8719,7 +8723,7 @@
         <v>-0.26194320300000001</v>
       </c>
       <c r="BG34" s="3">
-        <v>9000</v>
+        <v>0.28091731199999997</v>
       </c>
       <c r="BH34" s="3">
         <v>-4.3663440000000003E-3</v>
@@ -8952,7 +8956,7 @@
         <v>-0.944448552</v>
       </c>
       <c r="BG35" s="3">
-        <v>9000</v>
+        <v>0.36712641200000001</v>
       </c>
       <c r="BH35" s="3">
         <v>-5.9768210000000002E-3</v>
@@ -9185,7 +9189,7 @@
         <v>0.265394613</v>
       </c>
       <c r="BG36" s="3">
-        <v>9000</v>
+        <v>0.23002478600000001</v>
       </c>
       <c r="BH36" s="3">
         <v>-3.1072640000000002E-3</v>
@@ -9418,7 +9422,7 @@
         <v>-4.2589596739999998</v>
       </c>
       <c r="BG37" s="3">
-        <v>9000</v>
+        <v>0.64537777799999996</v>
       </c>
       <c r="BH37" s="3">
         <v>-1.1632326E-2</v>
@@ -9651,7 +9655,7 @@
         <v>-1.878381238</v>
       </c>
       <c r="BG38" s="3">
-        <v>9000</v>
+        <v>0.28497573500000001</v>
       </c>
       <c r="BH38" s="3">
         <v>-4.4761549999999999E-3</v>
@@ -9884,7 +9888,7 @@
         <v>-2.395842016</v>
       </c>
       <c r="BG39" s="3">
-        <v>9000</v>
+        <v>0.40634153699999997</v>
       </c>
       <c r="BH39" s="3">
         <v>-7.2741960000000001E-3</v>
@@ -10117,7 +10121,7 @@
         <v>-0.66670964899999996</v>
       </c>
       <c r="BG40" s="3">
-        <v>9000</v>
+        <v>0.26753637699999999</v>
       </c>
       <c r="BH40" s="3">
         <v>-4.4307629999999999E-3</v>
@@ -10350,7 +10354,7 @@
         <v>-1.652969014</v>
       </c>
       <c r="BG41" s="3">
-        <v>9000</v>
+        <v>0.37093864900000001</v>
       </c>
       <c r="BH41" s="3">
         <v>-6.0068029999999998E-3</v>
@@ -10816,7 +10820,7 @@
         <v>-1.523318739</v>
       </c>
       <c r="BG43" s="3">
-        <v>9000</v>
+        <v>0.25610587099999998</v>
       </c>
       <c r="BH43" s="3">
         <v>-3.5544489999999999E-3</v>
@@ -11515,7 +11519,7 @@
         <v>-0.129684415</v>
       </c>
       <c r="BG46" s="3">
-        <v>9000</v>
+        <v>0.14628453299999999</v>
       </c>
       <c r="BH46" s="3">
         <v>-1.9825509999999999E-3</v>
@@ -11748,7 +11752,7 @@
         <v>-2.4748219389999999</v>
       </c>
       <c r="BG47" s="3">
-        <v>9000</v>
+        <v>0.32612362900000003</v>
       </c>
       <c r="BH47" s="3">
         <v>-4.9000659999999998E-3</v>
@@ -11981,7 +11985,7 @@
         <v>-1.624700085</v>
       </c>
       <c r="BG48" s="3">
-        <v>9000</v>
+        <v>0.24026043</v>
       </c>
       <c r="BH48" s="3">
         <v>-3.3182680000000001E-3</v>
@@ -12214,7 +12218,7 @@
         <v>-2.2748063890000001</v>
       </c>
       <c r="BG49" s="3">
-        <v>9000</v>
+        <v>0.30782482100000003</v>
       </c>
       <c r="BH49" s="3">
         <v>-4.1819509999999997E-3</v>
@@ -12447,7 +12451,7 @@
         <v>-0.69810856899999996</v>
       </c>
       <c r="BG50" s="3">
-        <v>9000</v>
+        <v>0.126775375</v>
       </c>
       <c r="BH50" s="3">
         <v>-1.3583880000000001E-3</v>
@@ -12680,7 +12684,7 @@
         <v>-0.84938756599999998</v>
       </c>
       <c r="BG51" s="3">
-        <v>9000</v>
+        <v>0.17480823000000001</v>
       </c>
       <c r="BH51" s="3">
         <v>-2.0238420000000001E-3</v>
@@ -12913,7 +12917,7 @@
         <v>4.2399758000000003E-2</v>
       </c>
       <c r="BG52" s="3">
-        <v>9000</v>
+        <v>0.18567600400000001</v>
       </c>
       <c r="BH52" s="3">
         <v>-1.901079E-3</v>
@@ -13612,7 +13616,7 @@
         <v>-1.2372674749999999</v>
       </c>
       <c r="BG55" s="3">
-        <v>9000</v>
+        <v>0.228792987</v>
       </c>
       <c r="BH55" s="3">
         <v>-2.602236E-3</v>
@@ -13845,7 +13849,7 @@
         <v>-1.338345055</v>
       </c>
       <c r="BG56" s="3">
-        <v>9000</v>
+        <v>0.159708658</v>
       </c>
       <c r="BH56" s="3">
         <v>-1.454934E-3</v>
@@ -14311,7 +14315,7 @@
         <v>-2.8637498890000002</v>
       </c>
       <c r="BG58" s="3">
-        <v>9000</v>
+        <v>0.31663258999999999</v>
       </c>
       <c r="BH58" s="3">
         <v>-4.0236860000000003E-3</v>
@@ -14544,7 +14548,7 @@
         <v>-0.69324541200000001</v>
       </c>
       <c r="BG59" s="3">
-        <v>9000</v>
+        <v>0.27247167300000003</v>
       </c>
       <c r="BH59" s="3">
         <v>-3.5618109999999998E-3</v>
@@ -14777,7 +14781,7 @@
         <v>0.85265283800000002</v>
       </c>
       <c r="BG60" s="3">
-        <v>9000</v>
+        <v>0.13812226399999999</v>
       </c>
       <c r="BH60" s="3">
         <v>-1.1353310000000001E-3</v>
@@ -15010,7 +15014,7 @@
         <v>-1.7036469400000001</v>
       </c>
       <c r="BG61" s="3">
-        <v>9000</v>
+        <v>0.166436207</v>
       </c>
       <c r="BH61" s="3">
         <v>-1.4984289999999999E-3</v>
@@ -15243,7 +15247,7 @@
         <v>0.92360737699999995</v>
       </c>
       <c r="BG62" s="3">
-        <v>9000</v>
+        <v>0.105351033</v>
       </c>
       <c r="BH62" s="3">
         <v>-4.8948199999999996E-4</v>
@@ -15476,7 +15480,7 @@
         <v>-0.64983577199999998</v>
       </c>
       <c r="BG63" s="3">
-        <v>9000</v>
+        <v>0.220268035</v>
       </c>
       <c r="BH63" s="3">
         <v>-2.53857E-3</v>
@@ -15709,7 +15713,7 @@
         <v>-0.26297165300000003</v>
       </c>
       <c r="BG64" s="3">
-        <v>9000</v>
+        <v>0.25379967399999998</v>
       </c>
       <c r="BH64" s="3">
         <v>-3.3507430000000002E-3</v>
@@ -15942,7 +15946,7 @@
         <v>-0.53183253100000005</v>
       </c>
       <c r="BG65" s="3">
-        <v>9000</v>
+        <v>0.220165953</v>
       </c>
       <c r="BH65" s="3">
         <v>-3.0527250000000001E-3</v>
@@ -16175,7 +16179,7 @@
         <v>-0.55566249199999995</v>
       </c>
       <c r="BG66" s="3">
-        <v>9000</v>
+        <v>0.17945929599999999</v>
       </c>
       <c r="BH66" s="3">
         <v>-1.637342E-3</v>
@@ -16408,7 +16412,7 @@
         <v>0.30694127399999999</v>
       </c>
       <c r="BG67" s="3">
-        <v>9000</v>
+        <v>0.19131357500000001</v>
       </c>
       <c r="BH67" s="3">
         <v>-2.2768200000000001E-3</v>
@@ -16641,7 +16645,7 @@
         <v>1.480615673</v>
       </c>
       <c r="BG68" s="3">
-        <v>9000</v>
+        <v>0.10172318599999999</v>
       </c>
       <c r="BH68" s="3">
         <v>-2.38645E-4</v>
@@ -16874,7 +16878,7 @@
         <v>1.340252518</v>
       </c>
       <c r="BG69" s="3">
-        <v>9000</v>
+        <v>0.159149492</v>
       </c>
       <c r="BH69" s="3">
         <v>-1.680151E-3</v>
@@ -17107,7 +17111,7 @@
         <v>1.0227543960000001</v>
       </c>
       <c r="BG70" s="3">
-        <v>9000</v>
+        <v>0.188200796</v>
       </c>
       <c r="BH70" s="3">
         <v>-2.156748E-3</v>
@@ -17573,7 +17577,7 @@
         <v>1.388759909</v>
       </c>
       <c r="BG72" s="3">
-        <v>9000</v>
+        <v>0.13582108800000001</v>
       </c>
       <c r="BH72" s="3">
         <v>-1.782713E-3</v>
@@ -17806,7 +17810,7 @@
         <v>-0.99719810799999997</v>
       </c>
       <c r="BG73" s="3">
-        <v>9000</v>
+        <v>0.31800967899999999</v>
       </c>
       <c r="BH73" s="3">
         <v>-4.7655859999999996E-3</v>
@@ -18039,7 +18043,7 @@
         <v>1.7696027089999999</v>
       </c>
       <c r="BG74" s="3">
-        <v>9000</v>
+        <v>0.106215689</v>
       </c>
       <c r="BH74" s="3">
         <v>-1.1039719999999999E-3</v>
@@ -18272,7 +18276,7 @@
         <v>0.405354563</v>
       </c>
       <c r="BG75" s="3">
-        <v>9000</v>
+        <v>0.23962660799999999</v>
       </c>
       <c r="BH75" s="3">
         <v>-3.4094220000000001E-3</v>
@@ -18505,7 +18509,7 @@
         <v>0.249335999</v>
       </c>
       <c r="BG76" s="3">
-        <v>9000</v>
+        <v>0.23107805300000001</v>
       </c>
       <c r="BH76" s="3">
         <v>-3.4946930000000001E-3</v>
@@ -18738,7 +18742,7 @@
         <v>-2.394263622</v>
       </c>
       <c r="BG77" s="3">
-        <v>9000</v>
+        <v>0.44194383599999998</v>
       </c>
       <c r="BH77" s="3">
         <v>-7.2776430000000003E-3</v>
@@ -18971,7 +18975,7 @@
         <v>-2.2749144569999999</v>
       </c>
       <c r="BG78" s="3">
-        <v>9000</v>
+        <v>0.43160820700000002</v>
       </c>
       <c r="BH78" s="3">
         <v>-7.2248820000000002E-3</v>
@@ -19204,7 +19208,7 @@
         <v>-1.628587308</v>
       </c>
       <c r="BG79" s="3">
-        <v>9000</v>
+        <v>0.43553438799999999</v>
       </c>
       <c r="BH79" s="3">
         <v>-7.3950209999999999E-3</v>
@@ -19437,7 +19441,7 @@
         <v>0.114479966</v>
       </c>
       <c r="BG80" s="3">
-        <v>9000</v>
+        <v>0.24633184</v>
       </c>
       <c r="BH80" s="3">
         <v>-3.7039529999999998E-3</v>
@@ -19903,7 +19907,7 @@
         <v>0.61436996099999996</v>
       </c>
       <c r="BG82" s="3">
-        <v>9000</v>
+        <v>0.21832274300000001</v>
       </c>
       <c r="BH82" s="3">
         <v>-3.1437330000000001E-3</v>
@@ -20136,7 +20140,7 @@
         <v>-0.36623000900000002</v>
       </c>
       <c r="BG83" s="3">
-        <v>9000</v>
+        <v>0.24502077</v>
       </c>
       <c r="BH83" s="3">
         <v>-3.6205769999999998E-3</v>
@@ -20369,7 +20373,7 @@
         <v>-0.14987403399999999</v>
       </c>
       <c r="BG84" s="3">
-        <v>9000</v>
+        <v>0.176216607</v>
       </c>
       <c r="BH84" s="3">
         <v>-2.2098180000000001E-3</v>
@@ -20602,7 +20606,7 @@
         <v>-0.12264802499999999</v>
       </c>
       <c r="BG85" s="3">
-        <v>9000</v>
+        <v>0.236724289</v>
       </c>
       <c r="BH85" s="3">
         <v>-3.5017270000000001E-3</v>
@@ -20835,7 +20839,7 @@
         <v>-0.59763221300000002</v>
       </c>
       <c r="BG86" s="3">
-        <v>9000</v>
+        <v>0.20414400799999999</v>
       </c>
       <c r="BH86" s="3">
         <v>-2.9102799999999999E-3</v>
@@ -21068,7 +21072,7 @@
         <v>-1.7587343600000001</v>
       </c>
       <c r="BG87" s="3">
-        <v>9000</v>
+        <v>0.26532636999999998</v>
       </c>
       <c r="BH87" s="3">
         <v>-3.6528979999999999E-3</v>
@@ -21301,7 +21305,7 @@
         <v>-2.721941084</v>
       </c>
       <c r="BG88" s="3">
-        <v>9000</v>
+        <v>0.24219797200000001</v>
       </c>
       <c r="BH88" s="3">
         <v>-2.6083809999999999E-3</v>
@@ -21534,7 +21538,7 @@
         <v>-1.1136857659999999</v>
       </c>
       <c r="BG89" s="3">
-        <v>9000</v>
+        <v>0.201108438</v>
       </c>
       <c r="BH89" s="3">
         <v>-2.9255470000000001E-3</v>
@@ -21767,7 +21771,7 @@
         <v>3.49801E-2</v>
       </c>
       <c r="BG90" s="3">
-        <v>9000</v>
+        <v>0.11779458399999999</v>
       </c>
       <c r="BH90" s="3">
         <v>-1.1573029999999999E-3</v>
@@ -22699,7 +22703,7 @@
         <v>-0.85536352800000004</v>
       </c>
       <c r="BG94" s="3">
-        <v>9000</v>
+        <v>0.29598086499999998</v>
       </c>
       <c r="BH94" s="3">
         <v>-4.4567399999999998E-3</v>
@@ -22932,7 +22936,7 @@
         <v>-1.3426689249999999</v>
       </c>
       <c r="BG95" s="3">
-        <v>9000</v>
+        <v>0.38040138000000001</v>
       </c>
       <c r="BH95" s="3">
         <v>-6.082563E-3</v>
@@ -23398,7 +23402,7 @@
         <v>-1.140879843</v>
       </c>
       <c r="BG97" s="3">
-        <v>9000</v>
+        <v>0.274498034</v>
       </c>
       <c r="BH97" s="3">
         <v>-4.5266899999999999E-3</v>
@@ -23864,7 +23868,7 @@
         <v>-0.16292273700000001</v>
       </c>
       <c r="BG99" s="3">
-        <v>9000</v>
+        <v>0.266273447</v>
       </c>
       <c r="BH99" s="3">
         <v>-4.1157900000000002E-3</v>
@@ -24097,7 +24101,7 @@
         <v>-0.74532165900000003</v>
       </c>
       <c r="BG100" s="3">
-        <v>9000</v>
+        <v>0.32101680999999999</v>
       </c>
       <c r="BH100" s="3">
         <v>-4.7567119999999997E-3</v>
@@ -24796,7 +24800,7 @@
         <v>-1.810900687</v>
       </c>
       <c r="BG103" s="3">
-        <v>9000</v>
+        <v>0.28370081699999999</v>
       </c>
       <c r="BH103" s="3">
         <v>-3.4248299999999998E-3</v>
@@ -25728,7 +25732,7 @@
         <v>0.222395654</v>
       </c>
       <c r="BG107" s="3">
-        <v>9000</v>
+        <v>0.251426804</v>
       </c>
       <c r="BH107" s="3">
         <v>-3.422834E-3</v>
@@ -25961,7 +25965,7 @@
         <v>1.7296992920000001</v>
       </c>
       <c r="BG108" s="3">
-        <v>9000</v>
+        <v>0.11572171000000001</v>
       </c>
       <c r="BH108" s="3">
         <v>-6.8026999999999996E-4</v>
@@ -26194,7 +26198,7 @@
         <v>-0.797716274</v>
       </c>
       <c r="BG109" s="3">
-        <v>9000</v>
+        <v>0.29521346199999998</v>
       </c>
       <c r="BH109" s="3">
         <v>-3.795517E-3</v>
@@ -26427,7 +26431,7 @@
         <v>-3.4242838999999997E-2</v>
       </c>
       <c r="BG110" s="3">
-        <v>9000</v>
+        <v>0.249135786</v>
       </c>
       <c r="BH110" s="3">
         <v>-3.0524189999999998E-3</v>
@@ -26660,7 +26664,7 @@
         <v>1.292386043</v>
       </c>
       <c r="BG111" s="3">
-        <v>9000</v>
+        <v>0.115241516</v>
       </c>
       <c r="BH111" s="3">
         <v>-4.7712399999999999E-4</v>
@@ -28990,7 +28994,7 @@
         <v>0.92107340299999996</v>
       </c>
       <c r="BG121" s="3">
-        <v>9000</v>
+        <v>0.16503549100000001</v>
       </c>
       <c r="BH121" s="3">
         <v>-1.36892E-3</v>
@@ -29223,7 +29227,7 @@
         <v>0.43356012999999999</v>
       </c>
       <c r="BG122" s="3">
-        <v>9000</v>
+        <v>0.182051828</v>
       </c>
       <c r="BH122" s="3">
         <v>-1.6735700000000001E-3</v>
@@ -29456,7 +29460,7 @@
         <v>0.80021146899999995</v>
       </c>
       <c r="BG123" s="3">
-        <v>9000</v>
+        <v>0.109945802</v>
       </c>
       <c r="BH123" s="3">
         <v>-4.9486199999999999E-4</v>
@@ -29689,7 +29693,7 @@
         <v>7.2024106000000004E-2</v>
       </c>
       <c r="BG124" s="3">
-        <v>9000</v>
+        <v>0.201414707</v>
       </c>
       <c r="BH124" s="3">
         <v>-1.9089280000000001E-3</v>
@@ -29922,7 +29926,7 @@
         <v>0.56546323799999998</v>
       </c>
       <c r="BG125" s="3">
-        <v>9000</v>
+        <v>0.22543281900000001</v>
       </c>
       <c r="BH125" s="3">
         <v>-2.5545120000000001E-3</v>
@@ -30155,7 +30159,7 @@
         <v>0.23230192199999999</v>
       </c>
       <c r="BG126" s="3">
-        <v>9000</v>
+        <v>0.22814984999999999</v>
       </c>
       <c r="BH126" s="3">
         <v>-2.3924800000000002E-3</v>
@@ -30388,7 +30392,7 @@
         <v>0.83712252300000001</v>
       </c>
       <c r="BG127" s="3">
-        <v>9000</v>
+        <v>0.15806066399999999</v>
       </c>
       <c r="BH127" s="3">
         <v>-1.215676E-3</v>
@@ -30621,7 +30625,7 @@
         <v>-1.728030561</v>
       </c>
       <c r="BG128" s="3">
-        <v>9000</v>
+        <v>0.38522250699999999</v>
       </c>
       <c r="BH128" s="3">
         <v>-7.035098E-3</v>
@@ -30854,7 +30858,7 @@
         <v>1.8504821309999999</v>
       </c>
       <c r="BG129" s="3">
-        <v>9000</v>
+        <v>0.116927115</v>
       </c>
       <c r="BH129" s="3">
         <v>-1.3257049999999999E-3</v>
@@ -31087,7 +31091,7 @@
         <v>0.31323429400000002</v>
       </c>
       <c r="BG130" s="3">
-        <v>9000</v>
+        <v>0.122107673</v>
       </c>
       <c r="BH130" s="3">
         <v>-1.2500510000000001E-3</v>
@@ -31553,7 +31557,7 @@
         <v>1.088365673</v>
       </c>
       <c r="BG132" s="3">
-        <v>9000</v>
+        <v>0.18983275299999999</v>
       </c>
       <c r="BH132" s="3">
         <v>-2.520581E-3</v>
@@ -31786,7 +31790,7 @@
         <v>0.979013621</v>
       </c>
       <c r="BG133" s="3">
-        <v>9000</v>
+        <v>0.142731783</v>
       </c>
       <c r="BH133" s="3">
         <v>-1.6022E-3</v>
@@ -32252,7 +32256,7 @@
         <v>1.6429331199999999</v>
       </c>
       <c r="BG135" s="3">
-        <v>9000</v>
+        <v>0.131083962</v>
       </c>
       <c r="BH135" s="3">
         <v>-1.379836E-3</v>
@@ -32485,7 +32489,7 @@
         <v>2.1394651159999998</v>
       </c>
       <c r="BG136" s="3">
-        <v>9000</v>
+        <v>0.10950900700000001</v>
       </c>
       <c r="BH136" s="3">
         <v>-1.017434E-3</v>
@@ -32718,7 +32722,7 @@
         <v>-0.40314851699999998</v>
       </c>
       <c r="BG137" s="3">
-        <v>9000</v>
+        <v>0.16547805199999999</v>
       </c>
       <c r="BH137" s="3">
         <v>-2.0698079999999998E-3</v>
@@ -32951,7 +32955,7 @@
         <v>0.39912038999999999</v>
       </c>
       <c r="BG138" s="3">
-        <v>9000</v>
+        <v>0.18604593899999999</v>
       </c>
       <c r="BH138" s="3">
         <v>-2.4312359999999998E-3</v>
@@ -33184,7 +33188,7 @@
         <v>0.85462832600000005</v>
       </c>
       <c r="BG139" s="3">
-        <v>9000</v>
+        <v>0.168949348</v>
       </c>
       <c r="BH139" s="3">
         <v>-2.1228150000000001E-3</v>
@@ -33417,7 +33421,7 @@
         <v>0.35249443600000002</v>
       </c>
       <c r="BG140" s="3">
-        <v>9000</v>
+        <v>0.12723430799999999</v>
       </c>
       <c r="BH140" s="3">
         <v>-1.2360349999999999E-3</v>
@@ -33883,7 +33887,7 @@
         <v>0.83425381600000004</v>
       </c>
       <c r="BG142" s="3">
-        <v>9000</v>
+        <v>0.131325313</v>
       </c>
       <c r="BH142" s="3">
         <v>-1.1859189999999999E-3</v>
@@ -34116,7 +34120,7 @@
         <v>0.44571350399999998</v>
       </c>
       <c r="BG143" s="3">
-        <v>9000</v>
+        <v>0.109704275</v>
       </c>
       <c r="BH143" s="3">
         <v>-1.1076009999999999E-3</v>
@@ -34349,7 +34353,7 @@
         <v>0.20890022</v>
       </c>
       <c r="BG144" s="3">
-        <v>9000</v>
+        <v>0.17268778900000001</v>
       </c>
       <c r="BH144" s="3">
         <v>-2.451721E-3</v>
@@ -34582,7 +34586,7 @@
         <v>1.0306357260000001</v>
       </c>
       <c r="BG145" s="3">
-        <v>9000</v>
+        <v>0.11498174899999999</v>
       </c>
       <c r="BH145" s="3">
         <v>-1.482857E-3</v>
@@ -34815,7 +34819,7 @@
         <v>-0.32992777699999998</v>
       </c>
       <c r="BG146" s="3">
-        <v>9000</v>
+        <v>0.194713154</v>
       </c>
       <c r="BH146" s="3">
         <v>-2.9584199999999998E-3</v>
@@ -35048,7 +35052,7 @@
         <v>-0.72623506000000004</v>
       </c>
       <c r="BG147" s="3">
-        <v>9000</v>
+        <v>0.29477848200000001</v>
       </c>
       <c r="BH147" s="3">
         <v>-4.805747E-3</v>
@@ -35281,7 +35285,7 @@
         <v>1.237672018</v>
       </c>
       <c r="BG148" s="3">
-        <v>9000</v>
+        <v>7.2734223000000001E-2</v>
       </c>
       <c r="BH148" s="3">
         <v>-4.2749800000000001E-4</v>
@@ -35747,7 +35751,7 @@
         <v>1.0552276110000001</v>
       </c>
       <c r="BG150" s="3">
-        <v>9000</v>
+        <v>0.13614332300000001</v>
       </c>
       <c r="BH150" s="3">
         <v>-1.345871E-3</v>
@@ -36213,7 +36217,7 @@
         <v>0.74599883</v>
       </c>
       <c r="BG152" s="3">
-        <v>9000</v>
+        <v>9.6433932999999999E-2</v>
       </c>
       <c r="BH152" s="3">
         <v>-6.9890999999999996E-4</v>
@@ -36446,7 +36450,7 @@
         <v>1.333896827</v>
       </c>
       <c r="BG153" s="3">
-        <v>9000</v>
+        <v>8.0380966999999998E-2</v>
       </c>
       <c r="BH153" s="3">
         <v>-4.6904E-4</v>
@@ -36679,7 +36683,7 @@
         <v>1.525910178</v>
       </c>
       <c r="BG154" s="3">
-        <v>9000</v>
+        <v>9.0514069000000003E-2</v>
       </c>
       <c r="BH154" s="3">
         <v>-5.5627599999999997E-4</v>
@@ -36912,7 +36916,7 @@
         <v>1.4399066119999999</v>
       </c>
       <c r="BG155" s="3">
-        <v>9000</v>
+        <v>0.10620506</v>
       </c>
       <c r="BH155" s="3">
         <v>-7.7342600000000002E-4</v>
@@ -37145,7 +37149,7 @@
         <v>0.48070147699999999</v>
       </c>
       <c r="BG156" s="3">
-        <v>9000</v>
+        <v>0.21129720199999999</v>
       </c>
       <c r="BH156" s="3">
         <v>-2.585763E-3</v>
@@ -37378,7 +37382,7 @@
         <v>0.61739967900000003</v>
       </c>
       <c r="BG157" s="3">
-        <v>9000</v>
+        <v>0.15926891600000001</v>
       </c>
       <c r="BH157" s="3">
         <v>-1.720053E-3</v>
@@ -37611,7 +37615,7 @@
         <v>-0.75643180799999998</v>
       </c>
       <c r="BG158" s="3">
-        <v>9000</v>
+        <v>0.25836721800000001</v>
       </c>
       <c r="BH158" s="3">
         <v>-3.2994750000000001E-3</v>
@@ -37844,7 +37848,7 @@
         <v>0.30309184900000002</v>
       </c>
       <c r="BG159" s="3">
-        <v>9000</v>
+        <v>0.109246468</v>
       </c>
       <c r="BH159" s="3">
         <v>-1.2455700000000001E-3</v>
@@ -38077,7 +38081,7 @@
         <v>0.71631802499999997</v>
       </c>
       <c r="BG160" s="3">
-        <v>9000</v>
+        <v>0.110262558</v>
       </c>
       <c r="BH160" s="3">
         <v>-1.1790259999999999E-3</v>
@@ -38310,7 +38314,7 @@
         <v>1.41270031</v>
       </c>
       <c r="BG161" s="3">
-        <v>9000</v>
+        <v>4.3039792E-2</v>
       </c>
       <c r="BH161" s="3">
         <v>-1.20532E-4</v>
@@ -38543,7 +38547,7 @@
         <v>0.71531594799999998</v>
       </c>
       <c r="BG162" s="3">
-        <v>9000</v>
+        <v>0.181064582</v>
       </c>
       <c r="BH162" s="3">
         <v>-2.6008450000000001E-3</v>
@@ -38776,7 +38780,7 @@
         <v>0.66466441499999995</v>
       </c>
       <c r="BG163" s="3">
-        <v>9000</v>
+        <v>0.12866001599999999</v>
       </c>
       <c r="BH163" s="3">
         <v>-1.6933390000000001E-3</v>
@@ -39009,7 +39013,7 @@
         <v>4.6092466999999998E-2</v>
       </c>
       <c r="BG164" s="3">
-        <v>9000</v>
+        <v>0.161055955</v>
       </c>
       <c r="BH164" s="3">
         <v>-2.2567339999999998E-3</v>
@@ -39475,7 +39479,7 @@
         <v>1.465646096</v>
       </c>
       <c r="BG166" s="3">
-        <v>9000</v>
+        <v>7.9043094999999994E-2</v>
       </c>
       <c r="BH166" s="3">
         <v>-5.3166800000000001E-4</v>
@@ -39708,7 +39712,7 @@
         <v>1.758085457</v>
       </c>
       <c r="BG167" s="3">
-        <v>9000</v>
+        <v>8.8021041999999994E-2</v>
       </c>
       <c r="BH167" s="3">
         <v>-5.2758799999999995E-4</v>
@@ -39941,7 +39945,7 @@
         <v>-4.5282019999999999E-2</v>
       </c>
       <c r="BG168" s="3">
-        <v>9000</v>
+        <v>0.14450842899999999</v>
       </c>
       <c r="BH168" s="3">
         <v>-1.4128840000000001E-3</v>
@@ -40174,7 +40178,7 @@
         <v>0.20651919899999999</v>
       </c>
       <c r="BG169" s="3">
-        <v>9000</v>
+        <v>0.22157456</v>
       </c>
       <c r="BH169" s="3">
         <v>-2.7730849999999998E-3</v>
@@ -40407,7 +40411,7 @@
         <v>0.68127059499999998</v>
       </c>
       <c r="BG170" s="3">
-        <v>9000</v>
+        <v>0.116666292</v>
       </c>
       <c r="BH170" s="3">
         <v>-1.0273979999999999E-3</v>
@@ -40640,7 +40644,7 @@
         <v>1.3907960539999999</v>
       </c>
       <c r="BG171" s="3">
-        <v>9000</v>
+        <v>0.126526271</v>
       </c>
       <c r="BH171" s="3">
         <v>-1.057005E-3</v>
@@ -41106,7 +41110,7 @@
         <v>1.240211441</v>
       </c>
       <c r="BG173" s="3">
-        <v>9000</v>
+        <v>0.13626037599999999</v>
       </c>
       <c r="BH173" s="3">
         <v>-1.191325E-3</v>
@@ -41339,7 +41343,7 @@
         <v>1.2613723859999999</v>
       </c>
       <c r="BG174" s="3">
-        <v>9000</v>
+        <v>7.6823294E-2</v>
       </c>
       <c r="BH174" s="6">
         <v>-4.5599999999999997E-5</v>
@@ -41572,7 +41576,7 @@
         <v>0.91392817500000001</v>
       </c>
       <c r="BG175" s="3">
-        <v>9000</v>
+        <v>6.9929241000000003E-2</v>
       </c>
       <c r="BH175" s="3">
         <v>-3.2379899999999999E-4</v>
@@ -41805,7 +41809,7 @@
         <v>0.71899884199999997</v>
       </c>
       <c r="BG176" s="3">
-        <v>9000</v>
+        <v>0.219117756</v>
       </c>
       <c r="BH176" s="3">
         <v>-3.3168400000000002E-3</v>
@@ -42038,7 +42042,7 @@
         <v>1.4734543339999999</v>
       </c>
       <c r="BG177" s="3">
-        <v>9000</v>
+        <v>0.14525037299999999</v>
       </c>
       <c r="BH177" s="3">
         <v>-1.938836E-3</v>
@@ -42271,7 +42275,7 @@
         <v>-0.29255368900000001</v>
       </c>
       <c r="BG178" s="3">
-        <v>9000</v>
+        <v>0.21469254900000001</v>
       </c>
       <c r="BH178" s="3">
         <v>-2.7490629999999999E-3</v>
@@ -42504,7 +42508,7 @@
         <v>0.53053390499999997</v>
       </c>
       <c r="BG179" s="3">
-        <v>9000</v>
+        <v>0.21612794599999999</v>
       </c>
       <c r="BH179" s="3">
         <v>-3.1415620000000001E-3</v>
@@ -42737,7 +42741,7 @@
         <v>1.47665742</v>
       </c>
       <c r="BG180" s="3">
-        <v>9000</v>
+        <v>0.13163856199999999</v>
       </c>
       <c r="BH180" s="3">
         <v>-1.5317799999999999E-3</v>
@@ -42970,7 +42974,7 @@
         <v>1.9081455380000001</v>
       </c>
       <c r="BG181" s="3">
-        <v>9000</v>
+        <v>0.112546117</v>
       </c>
       <c r="BH181" s="3">
         <v>-1.1461900000000001E-3</v>
@@ -43203,7 +43207,7 @@
         <v>1.018398369</v>
       </c>
       <c r="BG182" s="3">
-        <v>9000</v>
+        <v>0.12947049699999999</v>
       </c>
       <c r="BH182" s="3">
         <v>-1.2876330000000001E-3</v>
@@ -43669,7 +43673,7 @@
         <v>0.41754906600000002</v>
       </c>
       <c r="BG184" s="3">
-        <v>9000</v>
+        <v>0.15652162</v>
       </c>
       <c r="BH184" s="3">
         <v>-1.8034590000000001E-3</v>
@@ -43902,7 +43906,7 @@
         <v>1.1974575190000001</v>
       </c>
       <c r="BG185" s="3">
-        <v>9000</v>
+        <v>0.20499784800000001</v>
       </c>
       <c r="BH185" s="3">
         <v>-2.7741409999999999E-3</v>
@@ -44135,7 +44139,7 @@
         <v>0.62998584999999996</v>
       </c>
       <c r="BG186" s="3">
-        <v>9000</v>
+        <v>0.112899949</v>
       </c>
       <c r="BH186" s="3">
         <v>-9.8814299999999992E-4</v>
@@ -44368,7 +44372,7 @@
         <v>1.40736251</v>
       </c>
       <c r="BG187" s="3">
-        <v>9000</v>
+        <v>8.3278560000000001E-2</v>
       </c>
       <c r="BH187" s="3">
         <v>-4.3522800000000001E-4</v>
@@ -44601,7 +44605,7 @@
         <v>1.295555641</v>
       </c>
       <c r="BG188" s="3">
-        <v>9000</v>
+        <v>0.101072517</v>
       </c>
       <c r="BH188" s="3">
         <v>-7.2368200000000001E-4</v>
@@ -44834,7 +44838,7 @@
         <v>1.1288668449999999</v>
       </c>
       <c r="BG189" s="3">
-        <v>9000</v>
+        <v>0.105511697</v>
       </c>
       <c r="BH189" s="3">
         <v>-8.5447699999999997E-4</v>
@@ -45067,7 +45071,7 @@
         <v>-8.5456545999999994E-2</v>
       </c>
       <c r="BG190" s="3">
-        <v>9000</v>
+        <v>0.26244385100000001</v>
       </c>
       <c r="BH190" s="3">
         <v>-3.9375319999999997E-3</v>
@@ -45300,7 +45304,7 @@
         <v>-0.75502193900000003</v>
       </c>
       <c r="BG191" s="3">
-        <v>9000</v>
+        <v>0.29379567099999998</v>
       </c>
       <c r="BH191" s="3">
         <v>-4.4437139999999997E-3</v>
@@ -45766,7 +45770,7 @@
         <v>1.2231262220000001</v>
       </c>
       <c r="BG193" s="3">
-        <v>9000</v>
+        <v>9.5651534999999996E-2</v>
       </c>
       <c r="BH193" s="3">
         <v>-3.4141E-4</v>
@@ -45999,7 +46003,7 @@
         <v>0.74730372899999997</v>
       </c>
       <c r="BG194" s="3">
-        <v>9000</v>
+        <v>0.195344033</v>
       </c>
       <c r="BH194" s="3">
         <v>-2.2906070000000001E-3</v>
@@ -46232,7 +46236,7 @@
         <v>0.94857218300000001</v>
       </c>
       <c r="BG195" s="3">
-        <v>9000</v>
+        <v>0.106225185</v>
       </c>
       <c r="BH195" s="3">
         <v>-8.4884299999999995E-4</v>
@@ -46465,7 +46469,7 @@
         <v>1.917975102</v>
       </c>
       <c r="BG196" s="3">
-        <v>9000</v>
+        <v>0.100072992</v>
       </c>
       <c r="BH196" s="3">
         <v>-9.2872600000000005E-4</v>
@@ -46698,7 +46702,7 @@
         <v>1.367046019</v>
       </c>
       <c r="BG197" s="3">
-        <v>9000</v>
+        <v>0.11005294</v>
       </c>
       <c r="BH197" s="3">
         <v>-9.1347100000000001E-4</v>
@@ -47863,7 +47867,7 @@
         <v>-0.115561233</v>
       </c>
       <c r="BG202" s="3">
-        <v>9000</v>
+        <v>0.16183204300000001</v>
       </c>
       <c r="BH202" s="3">
         <v>-1.4163369999999999E-3</v>
@@ -48096,7 +48100,7 @@
         <v>-0.93173493699999999</v>
       </c>
       <c r="BG203" s="3">
-        <v>9000</v>
+        <v>0.33872820399999998</v>
       </c>
       <c r="BH203" s="3">
         <v>-5.0616840000000003E-3</v>
@@ -48329,7 +48333,7 @@
         <v>-2.601736872</v>
       </c>
       <c r="BG204" s="3">
-        <v>9000</v>
+        <v>0.411087592</v>
       </c>
       <c r="BH204" s="3">
         <v>-5.9624810000000004E-3</v>
@@ -48562,7 +48566,7 @@
         <v>-0.23072886500000001</v>
       </c>
       <c r="BG205" s="3">
-        <v>9000</v>
+        <v>0.20055086799999999</v>
       </c>
       <c r="BH205" s="3">
         <v>-2.9695590000000001E-3</v>
@@ -49028,7 +49032,7 @@
         <v>-0.42339365600000001</v>
       </c>
       <c r="BG207" s="3">
-        <v>9000</v>
+        <v>0.22395468299999999</v>
       </c>
       <c r="BH207" s="3">
         <v>-3.6224989999999999E-3</v>
@@ -49261,7 +49265,7 @@
         <v>-1.273948332</v>
       </c>
       <c r="BG208" s="3">
-        <v>9000</v>
+        <v>0.294217901</v>
       </c>
       <c r="BH208" s="3">
         <v>-4.9457870000000001E-3</v>
@@ -49727,7 +49731,7 @@
         <v>-1.1305431509999999</v>
       </c>
       <c r="BG210" s="3">
-        <v>9000</v>
+        <v>0.17967688100000001</v>
       </c>
       <c r="BH210" s="3">
         <v>-2.638746E-3</v>
@@ -49960,7 +49964,7 @@
         <v>-1.2026673219999999</v>
       </c>
       <c r="BG211" s="3">
-        <v>9000</v>
+        <v>0.21665113999999999</v>
       </c>
       <c r="BH211" s="3">
         <v>-3.1870650000000002E-3</v>
@@ -50193,7 +50197,7 @@
         <v>0.17446901100000001</v>
       </c>
       <c r="BG212" s="3">
-        <v>9000</v>
+        <v>0.16005351800000001</v>
       </c>
       <c r="BH212" s="3">
         <v>-2.2987670000000002E-3</v>
@@ -50426,7 +50430,7 @@
         <v>-7.9941254000000003E-2</v>
       </c>
       <c r="BG213" s="3">
-        <v>9000</v>
+        <v>0.133333067</v>
       </c>
       <c r="BH213" s="3">
         <v>-1.652E-3</v>
@@ -51125,7 +51129,7 @@
         <v>1.0197366130000001</v>
       </c>
       <c r="BG216" s="3">
-        <v>9000</v>
+        <v>7.6115537999999996E-2</v>
       </c>
       <c r="BH216" s="3">
         <v>-5.7755899999999995E-4</v>
@@ -52057,7 +52061,7 @@
         <v>1.4800527889999999</v>
       </c>
       <c r="BG220" s="3">
-        <v>9000</v>
+        <v>0.120047106</v>
       </c>
       <c r="BH220" s="3">
         <v>-1.686711E-3</v>
@@ -52290,7 +52294,7 @@
         <v>-1.3294664490000001</v>
       </c>
       <c r="BG221" s="3">
-        <v>9000</v>
+        <v>0.29283103300000002</v>
       </c>
       <c r="BH221" s="3">
         <v>-4.1743689999999998E-3</v>
@@ -52756,7 +52760,7 @@
         <v>0.54934928500000002</v>
       </c>
       <c r="BG223" s="3">
-        <v>9000</v>
+        <v>0.235437166</v>
       </c>
       <c r="BH223" s="3">
         <v>-2.9983739999999998E-3</v>
@@ -52989,7 +52993,7 @@
         <v>1.1087802980000001</v>
       </c>
       <c r="BG224" s="3">
-        <v>9000</v>
+        <v>0.19601256</v>
       </c>
       <c r="BH224" s="3">
         <v>-2.331105E-3</v>
@@ -53222,7 +53226,7 @@
         <v>-0.899664625</v>
       </c>
       <c r="BG225" s="3">
-        <v>9000</v>
+        <v>0.31387592399999997</v>
       </c>
       <c r="BH225" s="3">
         <v>-4.3116459999999997E-3</v>
@@ -53455,7 +53459,7 @@
         <v>-0.74729843200000001</v>
       </c>
       <c r="BG226" s="3">
-        <v>9000</v>
+        <v>0.26852454599999998</v>
       </c>
       <c r="BH226" s="3">
         <v>-4.142237E-3</v>
@@ -53688,7 +53692,7 @@
         <v>0.65414580200000005</v>
       </c>
       <c r="BG227" s="3">
-        <v>9000</v>
+        <v>0.19785356200000001</v>
       </c>
       <c r="BH227" s="3">
         <v>-2.4102030000000001E-3</v>
@@ -53921,7 +53925,7 @@
         <v>-0.46038963900000002</v>
       </c>
       <c r="BG228" s="3">
-        <v>9000</v>
+        <v>0.22670958399999999</v>
       </c>
       <c r="BH228" s="3">
         <v>-3.4127839999999999E-3</v>
@@ -54387,7 +54391,7 @@
         <v>0.37697667400000001</v>
       </c>
       <c r="BG230" s="3">
-        <v>9000</v>
+        <v>0.21571364700000001</v>
       </c>
       <c r="BH230" s="3">
         <v>-2.5873770000000001E-3</v>
@@ -54620,7 +54624,7 @@
         <v>-0.76720861900000004</v>
       </c>
       <c r="BG231" s="3">
-        <v>9000</v>
+        <v>0.26623566799999998</v>
       </c>
       <c r="BH231" s="3">
         <v>-3.0075779999999999E-3</v>
@@ -54853,7 +54857,7 @@
         <v>1.17451587</v>
       </c>
       <c r="BG232" s="3">
-        <v>9000</v>
+        <v>0.15169848599999999</v>
       </c>
       <c r="BH232" s="3">
         <v>-1.299276E-3</v>
@@ -55086,7 +55090,7 @@
         <v>-0.26252763699999998</v>
       </c>
       <c r="BG233" s="3">
-        <v>9000</v>
+        <v>0.23488904299999999</v>
       </c>
       <c r="BH233" s="3">
         <v>-2.4719350000000002E-3</v>
@@ -55319,7 +55323,7 @@
         <v>1.1703695160000001</v>
       </c>
       <c r="BG234" s="3">
-        <v>9000</v>
+        <v>0.13651319000000001</v>
       </c>
       <c r="BH234" s="3">
         <v>-7.6422000000000003E-4</v>
@@ -55785,7 +55789,7 @@
         <v>-2.6130837520000001</v>
       </c>
       <c r="BG236" s="3">
-        <v>9000</v>
+        <v>0.25467903600000003</v>
       </c>
       <c r="BH236" s="3">
         <v>-4.0189910000000004E-3</v>
@@ -56018,7 +56022,7 @@
         <v>-1.567047764</v>
       </c>
       <c r="BG237" s="3">
-        <v>9000</v>
+        <v>0.16095743100000001</v>
       </c>
       <c r="BH237" s="3">
         <v>-1.9719719999999998E-3</v>
@@ -56251,7 +56255,7 @@
         <v>-1.814156444</v>
       </c>
       <c r="BG238" s="3">
-        <v>9000</v>
+        <v>0.181780202</v>
       </c>
       <c r="BH238" s="3">
         <v>-2.5597689999999999E-3</v>
@@ -56717,7 +56721,7 @@
         <v>-2.0555317460000002</v>
       </c>
       <c r="BG240" s="3">
-        <v>9000</v>
+        <v>0.336544607</v>
       </c>
       <c r="BH240" s="3">
         <v>-5.4958790000000004E-3</v>
@@ -56950,7 +56954,7 @@
         <v>-3.5236178420000002</v>
       </c>
       <c r="BG241" s="3">
-        <v>9000</v>
+        <v>0.49163240499999999</v>
       </c>
       <c r="BH241" s="3">
         <v>-8.5322479999999992E-3</v>
@@ -57183,7 +57187,7 @@
         <v>-1.1632722200000001</v>
       </c>
       <c r="BG242" s="3">
-        <v>9000</v>
+        <v>0.27242174600000002</v>
       </c>
       <c r="BH242" s="3">
         <v>-4.352547E-3</v>
@@ -57416,7 +57420,7 @@
         <v>-0.171207161</v>
       </c>
       <c r="BG243" s="3">
-        <v>9000</v>
+        <v>0.19245748200000001</v>
       </c>
       <c r="BH243" s="3">
         <v>-2.9602489999999999E-3</v>
@@ -57649,7 +57653,7 @@
         <v>2.8720251819999998</v>
       </c>
       <c r="BG244" s="3">
-        <v>9000</v>
+        <v>5.3722803999999999E-2</v>
       </c>
       <c r="BH244" s="3">
         <v>-1.093508E-3</v>
@@ -57882,7 +57886,7 @@
         <v>1.608844272</v>
       </c>
       <c r="BG245" s="3">
-        <v>9000</v>
+        <v>9.7360484999999997E-2</v>
       </c>
       <c r="BH245" s="3">
         <v>-1.424984E-3</v>
@@ -58115,7 +58119,7 @@
         <v>1.1659648970000001</v>
       </c>
       <c r="BG246" s="3">
-        <v>9000</v>
+        <v>6.7768540000000002E-2</v>
       </c>
       <c r="BH246" s="3">
         <v>-8.1126799999999997E-4</v>
@@ -58581,7 +58585,7 @@
         <v>0.91626485499999999</v>
       </c>
       <c r="BG248" s="3">
-        <v>9000</v>
+        <v>9.8217999E-2</v>
       </c>
       <c r="BH248" s="3">
         <v>-1.1644750000000001E-3</v>
@@ -59047,7 +59051,7 @@
         <v>1.184399787</v>
       </c>
       <c r="BG250" s="3">
-        <v>9000</v>
+        <v>8.5456791000000004E-2</v>
       </c>
       <c r="BH250" s="3">
         <v>-1.309382E-3</v>
@@ -59513,7 +59517,7 @@
         <v>0.36420287800000001</v>
       </c>
       <c r="BG252" s="3">
-        <v>9000</v>
+        <v>0.18743636</v>
       </c>
       <c r="BH252" s="3">
         <v>-2.75691E-3</v>
@@ -59979,7 +59983,7 @@
         <v>2.0283030649999998</v>
       </c>
       <c r="BG254" s="3">
-        <v>9000</v>
+        <v>2.9443718000000001E-2</v>
       </c>
       <c r="BH254" s="3">
         <v>-3.9805199999999998E-4</v>
@@ -60445,7 +60449,7 @@
         <v>0.62918711900000002</v>
       </c>
       <c r="BG256" s="3">
-        <v>9000</v>
+        <v>0.138840821</v>
       </c>
       <c r="BH256" s="3">
         <v>-2.0471249999999999E-3</v>
@@ -60911,7 +60915,7 @@
         <v>1.5994911839999999</v>
       </c>
       <c r="BG258" s="3">
-        <v>9000</v>
+        <v>7.4662694000000002E-2</v>
       </c>
       <c r="BH258" s="3">
         <v>-7.6430300000000003E-4</v>
@@ -61144,7 +61148,7 @@
         <v>-0.599977859</v>
       </c>
       <c r="BG259" s="3">
-        <v>9000</v>
+        <v>0.16578890900000001</v>
       </c>
       <c r="BH259" s="3">
         <v>-2.2758069999999999E-3</v>
@@ -61610,7 +61614,7 @@
         <v>-0.14028997100000001</v>
       </c>
       <c r="BG261" s="3">
-        <v>9000</v>
+        <v>0.15901739500000001</v>
       </c>
       <c r="BH261" s="3">
         <v>-2.5223889999999999E-3</v>
@@ -62076,7 +62080,7 @@
         <v>-0.304432653</v>
       </c>
       <c r="BG263" s="3">
-        <v>9000</v>
+        <v>0.28989084100000001</v>
       </c>
       <c r="BH263" s="3">
         <v>-4.0946309999999996E-3</v>
@@ -62309,7 +62313,7 @@
         <v>0.82778261799999997</v>
       </c>
       <c r="BG264" s="3">
-        <v>9000</v>
+        <v>0.13261584300000001</v>
       </c>
       <c r="BH264" s="3">
         <v>-1.5894819999999999E-3</v>
@@ -62775,7 +62779,7 @@
         <v>0.38112519099999997</v>
       </c>
       <c r="BG266" s="3">
-        <v>9000</v>
+        <v>0.16371290999999999</v>
       </c>
       <c r="BH266" s="3">
         <v>-2.079277E-3</v>
@@ -63940,7 +63944,7 @@
         <v>-1.38463531</v>
       </c>
       <c r="BG271" s="3">
-        <v>9000</v>
+        <v>0.263954998</v>
       </c>
       <c r="BH271" s="3">
         <v>-3.788114E-3</v>
@@ -64173,7 +64177,7 @@
         <v>-1.0442324890000001</v>
       </c>
       <c r="BG272" s="3">
-        <v>9000</v>
+        <v>0.269873853</v>
       </c>
       <c r="BH272" s="3">
         <v>-3.8929049999999999E-3</v>
@@ -64639,7 +64643,7 @@
         <v>-1.514345381</v>
       </c>
       <c r="BG274" s="3">
-        <v>9000</v>
+        <v>0.28315093499999999</v>
       </c>
       <c r="BH274" s="3">
         <v>-4.054729E-3</v>
@@ -65338,7 +65342,7 @@
         <v>-0.22068315199999999</v>
       </c>
       <c r="BG277" s="3">
-        <v>9000</v>
+        <v>0.23528299599999999</v>
       </c>
       <c r="BH277" s="3">
         <v>-2.9569179999999998E-3</v>
@@ -65804,7 +65808,7 @@
         <v>-0.37339994999999998</v>
       </c>
       <c r="BG279" s="3">
-        <v>9000</v>
+        <v>0.26861634699999998</v>
       </c>
       <c r="BH279" s="3">
         <v>-3.7529690000000001E-3</v>
@@ -66037,7 +66041,7 @@
         <v>-0.16328313</v>
       </c>
       <c r="BG280" s="3">
-        <v>9000</v>
+        <v>0.17389877200000001</v>
       </c>
       <c r="BH280" s="3">
         <v>-1.5778649999999999E-3</v>
@@ -66270,7 +66274,7 @@
         <v>-1.257496078</v>
       </c>
       <c r="BG281" s="3">
-        <v>9000</v>
+        <v>0.30701709599999999</v>
       </c>
       <c r="BH281" s="3">
         <v>-4.1684670000000004E-3</v>
@@ -66503,7 +66507,7 @@
         <v>-0.93603605099999998</v>
       </c>
       <c r="BG282" s="3">
-        <v>9000</v>
+        <v>0.21567255799999999</v>
       </c>
       <c r="BH282" s="3">
         <v>-3.2499120000000002E-3</v>
@@ -66736,7 +66740,7 @@
         <v>2.0157804439999998</v>
       </c>
       <c r="BG283" s="3">
-        <v>9000</v>
+        <v>6.0973222000000001E-2</v>
       </c>
       <c r="BH283" s="3">
         <v>-1.587804E-3</v>
@@ -67202,7 +67206,7 @@
         <v>0.22548868699999999</v>
       </c>
       <c r="BG285" s="3">
-        <v>9000</v>
+        <v>9.7678413000000006E-2</v>
       </c>
       <c r="BH285" s="3">
         <v>-1.1265089999999999E-3</v>
@@ -67435,7 +67439,7 @@
         <v>-0.93998478699999999</v>
       </c>
       <c r="BG286" s="3">
-        <v>9000</v>
+        <v>0.26603586000000001</v>
       </c>
       <c r="BH286" s="3">
         <v>-4.4143489999999997E-3</v>
@@ -67901,7 +67905,7 @@
         <v>-0.506971744</v>
       </c>
       <c r="BG288" s="3">
-        <v>9000</v>
+        <v>0.24255810899999999</v>
       </c>
       <c r="BH288" s="3">
         <v>-3.205421E-3</v>
@@ -68134,7 +68138,7 @@
         <v>0.55635342099999996</v>
       </c>
       <c r="BG289" s="3">
-        <v>9000</v>
+        <v>0.16937633799999999</v>
       </c>
       <c r="BH289" s="3">
         <v>-1.8432100000000001E-3</v>
@@ -68367,7 +68371,7 @@
         <v>0.66452977099999999</v>
       </c>
       <c r="BG290" s="3">
-        <v>9000</v>
+        <v>0.15886098500000001</v>
       </c>
       <c r="BH290" s="3">
         <v>-1.7887319999999999E-3</v>
@@ -68600,7 +68604,7 @@
         <v>0.27813132000000002</v>
       </c>
       <c r="BG291" s="3">
-        <v>9000</v>
+        <v>0.101810041</v>
       </c>
       <c r="BH291" s="3">
         <v>-8.9483200000000003E-4</v>
@@ -68833,7 +68837,7 @@
         <v>0.13450174500000001</v>
       </c>
       <c r="BG292" s="3">
-        <v>9000</v>
+        <v>0.24921406400000001</v>
       </c>
       <c r="BH292" s="3">
         <v>-3.26239E-3</v>
@@ -69066,7 +69070,7 @@
         <v>0.26169242500000001</v>
       </c>
       <c r="BG293" s="3">
-        <v>9000</v>
+        <v>0.21754079400000001</v>
       </c>
       <c r="BH293" s="3">
         <v>-2.9354260000000001E-3</v>
@@ -69299,7 +69303,7 @@
         <v>-0.18414012699999999</v>
       </c>
       <c r="BG294" s="3">
-        <v>9000</v>
+        <v>0.25660453799999999</v>
       </c>
       <c r="BH294" s="3">
         <v>-3.4143329999999999E-3</v>
@@ -69532,7 +69536,7 @@
         <v>0.22251496700000001</v>
       </c>
       <c r="BG295" s="3">
-        <v>9000</v>
+        <v>0.26016553399999998</v>
       </c>
       <c r="BH295" s="3">
         <v>-3.7026070000000001E-3</v>
@@ -69765,7 +69769,7 @@
         <v>0.65195204299999998</v>
       </c>
       <c r="BG296" s="3">
-        <v>9000</v>
+        <v>0.19974630900000001</v>
       </c>
       <c r="BH296" s="3">
         <v>-2.3733819999999998E-3</v>
@@ -69998,7 +70002,7 @@
         <v>-1.0388796410000001</v>
       </c>
       <c r="BG297" s="3">
-        <v>9000</v>
+        <v>0.35599345700000001</v>
       </c>
       <c r="BH297" s="3">
         <v>-5.6220480000000001E-3</v>
@@ -70231,7 +70235,7 @@
         <v>0.70076696199999999</v>
       </c>
       <c r="BG298" s="3">
-        <v>9000</v>
+        <v>0.173768591</v>
       </c>
       <c r="BH298" s="3">
         <v>-1.724941E-3</v>
@@ -70464,7 +70468,7 @@
         <v>0.46893538099999998</v>
       </c>
       <c r="BG299" s="3">
-        <v>9000</v>
+        <v>0.237062891</v>
       </c>
       <c r="BH299" s="3">
         <v>-3.3514030000000002E-3</v>
@@ -70697,7 +70701,7 @@
         <v>-0.399877604</v>
       </c>
       <c r="BG300" s="3">
-        <v>9000</v>
+        <v>0.25631033800000003</v>
       </c>
       <c r="BH300" s="3">
         <v>-3.3339989999999998E-3</v>
@@ -70930,7 +70934,7 @@
         <v>0.736373477</v>
       </c>
       <c r="BG301" s="3">
-        <v>9000</v>
+        <v>-1.373839E-2</v>
       </c>
       <c r="BH301" s="3">
         <v>1.8836110000000001E-3</v>
@@ -71163,7 +71167,7 @@
         <v>-0.93801382700000002</v>
       </c>
       <c r="BG302" s="3">
-        <v>9000</v>
+        <v>0.29444932600000001</v>
       </c>
       <c r="BH302" s="3">
         <v>-3.96584E-3</v>
@@ -71396,7 +71400,7 @@
         <v>1.783568426</v>
       </c>
       <c r="BG303" s="3">
-        <v>9000</v>
+        <v>0.12508290899999999</v>
       </c>
       <c r="BH303" s="3">
         <v>-7.4131999999999996E-4</v>
@@ -71629,7 +71633,7 @@
         <v>1.8178242520000001</v>
       </c>
       <c r="BG304" s="3">
-        <v>9000</v>
+        <v>0.109344778</v>
       </c>
       <c r="BH304" s="3">
         <v>-4.6496299999999999E-4</v>
@@ -72095,7 +72099,7 @@
         <v>2.8846704929999998</v>
       </c>
       <c r="BG306" s="3">
-        <v>9000</v>
+        <v>5.2128239E-2</v>
       </c>
       <c r="BH306" s="6">
         <v>-9.8300000000000004E-5</v>
@@ -72328,7 +72332,7 @@
         <v>-0.47422408100000002</v>
       </c>
       <c r="BG307" s="3">
-        <v>9000</v>
+        <v>0.29233952200000002</v>
       </c>
       <c r="BH307" s="3">
         <v>-4.4070530000000002E-3</v>
@@ -72561,7 +72565,7 @@
         <v>0.40169304700000003</v>
       </c>
       <c r="BG308" s="3">
-        <v>9000</v>
+        <v>0.245826288</v>
       </c>
       <c r="BH308" s="3">
         <v>-3.026155E-3</v>
@@ -72794,7 +72798,7 @@
         <v>0.42289049899999998</v>
       </c>
       <c r="BG309" s="3">
-        <v>9000</v>
+        <v>0.23610336100000001</v>
       </c>
       <c r="BH309" s="3">
         <v>-3.2650359999999998E-3</v>
@@ -73027,7 +73031,7 @@
         <v>-0.99146302600000003</v>
       </c>
       <c r="BG310" s="3">
-        <v>9000</v>
+        <v>0.19951337</v>
       </c>
       <c r="BH310" s="3">
         <v>-3.0716530000000001E-3</v>
@@ -73260,7 +73264,7 @@
         <v>-9.1140051E-2</v>
       </c>
       <c r="BG311" s="3">
-        <v>9000</v>
+        <v>0.18240531900000001</v>
       </c>
       <c r="BH311" s="3">
         <v>-2.5580289999999999E-3</v>
@@ -73493,7 +73497,7 @@
         <v>-1.249246606</v>
       </c>
       <c r="BG312" s="3">
-        <v>9000</v>
+        <v>0.281288123</v>
       </c>
       <c r="BH312" s="3">
         <v>-4.2757539999999997E-3</v>
@@ -73726,7 +73730,7 @@
         <v>0.125062495</v>
       </c>
       <c r="BG313" s="3">
-        <v>9000</v>
+        <v>0.185287281</v>
       </c>
       <c r="BH313" s="3">
         <v>-2.981956E-3</v>
@@ -74192,7 +74196,7 @@
         <v>-0.48983537599999999</v>
       </c>
       <c r="BG315" s="3">
-        <v>9000</v>
+        <v>0.21056760499999999</v>
       </c>
       <c r="BH315" s="3">
         <v>-3.044948E-3</v>
@@ -74425,7 +74429,7 @@
         <v>-0.56902102600000004</v>
       </c>
       <c r="BG316" s="3">
-        <v>9000</v>
+        <v>0.22245758800000001</v>
       </c>
       <c r="BH316" s="3">
         <v>-3.469677E-3</v>
@@ -74658,7 +74662,7 @@
         <v>0.85116173100000003</v>
       </c>
       <c r="BG317" s="3">
-        <v>9000</v>
+        <v>0.17374329799999999</v>
       </c>
       <c r="BH317" s="3">
         <v>-2.0404300000000002E-3</v>
@@ -74891,7 +74895,7 @@
         <v>-1.7074113550000001</v>
       </c>
       <c r="BG318" s="3">
-        <v>9000</v>
+        <v>0.329551818</v>
       </c>
       <c r="BH318" s="3">
         <v>-4.9115280000000001E-3</v>
@@ -75124,7 +75128,7 @@
         <v>-0.42613766600000003</v>
       </c>
       <c r="BG319" s="3">
-        <v>9000</v>
+        <v>0.26863239700000002</v>
       </c>
       <c r="BH319" s="3">
         <v>-4.2415710000000004E-3</v>
@@ -75590,7 +75594,7 @@
         <v>0.25670488400000002</v>
       </c>
       <c r="BG321" s="3">
-        <v>9000</v>
+        <v>0.207089626</v>
       </c>
       <c r="BH321" s="3">
         <v>-2.6822259999999998E-3</v>
@@ -75823,7 +75827,7 @@
         <v>-1.738478067</v>
       </c>
       <c r="BG322" s="3">
-        <v>9000</v>
+        <v>0.25165200300000001</v>
       </c>
       <c r="BH322" s="3">
         <v>-2.6746959999999998E-3</v>
@@ -76056,7 +76060,7 @@
         <v>0.53235818999999995</v>
       </c>
       <c r="BG323" s="3">
-        <v>9000</v>
+        <v>0.19156723000000001</v>
       </c>
       <c r="BH323" s="3">
         <v>-2.2577159999999999E-3</v>
@@ -76289,7 +76293,7 @@
         <v>-0.32000092400000002</v>
       </c>
       <c r="BG324" s="3">
-        <v>9000</v>
+        <v>0.17844906699999999</v>
       </c>
       <c r="BH324" s="3">
         <v>-2.4591320000000002E-3</v>
@@ -76522,7 +76526,7 @@
         <v>0.31372213500000001</v>
       </c>
       <c r="BG325" s="3">
-        <v>9000</v>
+        <v>0.16612343700000001</v>
       </c>
       <c r="BH325" s="3">
         <v>-1.674165E-3</v>
@@ -76755,7 +76759,7 @@
         <v>0.315341765</v>
       </c>
       <c r="BG326" s="3">
-        <v>9000</v>
+        <v>0.204278864</v>
       </c>
       <c r="BH326" s="3">
         <v>-2.4921610000000001E-3</v>
@@ -76988,7 +76992,7 @@
         <v>-1.293832409</v>
       </c>
       <c r="BG327" s="3">
-        <v>9000</v>
+        <v>0.288921388</v>
       </c>
       <c r="BH327" s="3">
         <v>-5.1174660000000002E-3</v>
@@ -77221,7 +77225,7 @@
         <v>-1.682231874</v>
       </c>
       <c r="BG328" s="3">
-        <v>9000</v>
+        <v>0.32003130200000002</v>
       </c>
       <c r="BH328" s="3">
         <v>-5.2428010000000001E-3</v>
@@ -77454,7 +77458,7 @@
         <v>-0.127748579</v>
       </c>
       <c r="BG329" s="3">
-        <v>9000</v>
+        <v>0.215694203</v>
       </c>
       <c r="BH329" s="3">
         <v>-3.3633019999999999E-3</v>
@@ -77687,7 +77691,7 @@
         <v>0.60842571199999995</v>
       </c>
       <c r="BG330" s="3">
-        <v>9000</v>
+        <v>0.14669934000000001</v>
       </c>
       <c r="BH330" s="3">
         <v>-2.2347170000000002E-3</v>
@@ -77920,7 +77924,7 @@
         <v>0.66214473799999995</v>
       </c>
       <c r="BG331" s="3">
-        <v>9000</v>
+        <v>0.153664103</v>
       </c>
       <c r="BH331" s="3">
         <v>-2.3762610000000002E-3</v>
@@ -78153,7 +78157,7 @@
         <v>0.49263837900000002</v>
       </c>
       <c r="BG332" s="3">
-        <v>9000</v>
+        <v>0.17278216599999999</v>
       </c>
       <c r="BH332" s="3">
         <v>-2.6872710000000002E-3</v>
@@ -78386,7 +78390,7 @@
         <v>1.0130753269999999</v>
       </c>
       <c r="BG333" s="3">
-        <v>9000</v>
+        <v>0.14039478</v>
       </c>
       <c r="BH333" s="3">
         <v>-2.0855639999999998E-3</v>
@@ -78619,7 +78623,7 @@
         <v>0.646280152</v>
       </c>
       <c r="BG334" s="3">
-        <v>9000</v>
+        <v>0.16645534400000001</v>
       </c>
       <c r="BH334" s="3">
         <v>-2.7131770000000002E-3</v>
@@ -78852,7 +78856,7 @@
         <v>1.321365E-2</v>
       </c>
       <c r="BG335" s="3">
-        <v>9000</v>
+        <v>0.24318927500000001</v>
       </c>
       <c r="BH335" s="3">
         <v>-3.999664E-3</v>
@@ -79085,7 +79089,7 @@
         <v>0.94056754499999995</v>
       </c>
       <c r="BG336" s="3">
-        <v>9000</v>
+        <v>8.4406313999999996E-2</v>
       </c>
       <c r="BH336" s="3">
         <v>-1.1286530000000001E-3</v>
@@ -79318,7 +79322,7 @@
         <v>-0.138354372</v>
       </c>
       <c r="BG337" s="3">
-        <v>9000</v>
+        <v>0.19800762099999999</v>
       </c>
       <c r="BH337" s="3">
         <v>-2.833744E-3</v>
@@ -79551,7 +79555,7 @@
         <v>0.87179774899999996</v>
       </c>
       <c r="BG338" s="3">
-        <v>9000</v>
+        <v>0.15510446899999999</v>
       </c>
       <c r="BH338" s="3">
         <v>-2.2333750000000001E-3</v>
@@ -79784,7 +79788,7 @@
         <v>-2.4416401000000001E-2</v>
       </c>
       <c r="BG339" s="3">
-        <v>9000</v>
+        <v>0.16982287600000001</v>
       </c>
       <c r="BH339" s="3">
         <v>-2.4137339999999998E-3</v>
@@ -80017,7 +80021,7 @@
         <v>-0.170616927</v>
       </c>
       <c r="BG340" s="3">
-        <v>9000</v>
+        <v>0.163738141</v>
       </c>
       <c r="BH340" s="3">
         <v>-2.1842570000000002E-3</v>
@@ -80250,7 +80254,7 @@
         <v>1.1389233940000001</v>
       </c>
       <c r="BG341" s="3">
-        <v>9000</v>
+        <v>0.113584168</v>
       </c>
       <c r="BH341" s="3">
         <v>-1.5889879999999999E-3</v>
@@ -80483,7 +80487,7 @@
         <v>1.079376839</v>
       </c>
       <c r="BG342" s="3">
-        <v>9000</v>
+        <v>8.3395517000000002E-2</v>
       </c>
       <c r="BH342" s="3">
         <v>-1.0935109999999999E-3</v>
@@ -80949,7 +80953,7 @@
         <v>2.79558368</v>
       </c>
       <c r="BG344" s="3">
-        <v>9000</v>
+        <v>2.6690074000000001E-2</v>
       </c>
       <c r="BH344" s="3">
         <v>-2.4571499999999997E-4</v>
@@ -81182,7 +81186,7 @@
         <v>-0.81812895399999996</v>
       </c>
       <c r="BG345" s="3">
-        <v>9000</v>
+        <v>0.166958774</v>
       </c>
       <c r="BH345" s="3">
         <v>-2.6517229999999999E-3</v>
@@ -81648,7 +81652,7 @@
         <v>-0.52652606499999999</v>
       </c>
       <c r="BG347" s="3">
-        <v>9000</v>
+        <v>0.108186739</v>
       </c>
       <c r="BH347" s="3">
         <v>-1.469503E-3</v>
@@ -82114,7 +82118,7 @@
         <v>-0.58712534800000005</v>
       </c>
       <c r="BG349" s="3">
-        <v>9000</v>
+        <v>0.16890085599999999</v>
       </c>
       <c r="BH349" s="3">
         <v>-2.5432369999999998E-3</v>
@@ -82580,7 +82584,7 @@
         <v>0.68313224500000003</v>
       </c>
       <c r="BG351" s="3">
-        <v>9000</v>
+        <v>8.6427833999999995E-2</v>
       </c>
       <c r="BH351" s="3">
         <v>-1.041733E-3</v>
@@ -83046,7 +83050,7 @@
         <v>0.16114123999999999</v>
       </c>
       <c r="BG353" s="3">
-        <v>9000</v>
+        <v>0.13295099199999999</v>
       </c>
       <c r="BH353" s="3">
         <v>-2.0328870000000001E-3</v>
@@ -83279,7 +83283,7 @@
         <v>-0.73606415599999997</v>
       </c>
       <c r="BG354" s="3">
-        <v>9000</v>
+        <v>0.16111294400000001</v>
       </c>
       <c r="BH354" s="3">
         <v>-2.1461570000000001E-3</v>
@@ -83512,7 +83516,7 @@
         <v>8.3305332999999995E-2</v>
       </c>
       <c r="BG355" s="3">
-        <v>9000</v>
+        <v>0.19118101100000001</v>
       </c>
       <c r="BH355" s="3">
         <v>-2.9600809999999998E-3</v>
@@ -84444,7 +84448,7 @@
         <v>0.96236620900000003</v>
       </c>
       <c r="BG359" s="3">
-        <v>9000</v>
+        <v>0.14774143200000001</v>
       </c>
       <c r="BH359" s="3">
         <v>-2.2721159999999998E-3</v>
@@ -84677,7 +84681,7 @@
         <v>-0.67120075400000001</v>
       </c>
       <c r="BG360" s="3">
-        <v>9000</v>
+        <v>0.20857257700000001</v>
       </c>
       <c r="BH360" s="3">
         <v>-2.8897609999999998E-3</v>
@@ -85143,7 +85147,7 @@
         <v>0.55550188</v>
       </c>
       <c r="BG362" s="3">
-        <v>9000</v>
+        <v>0.12896384899999999</v>
       </c>
       <c r="BH362" s="3">
         <v>-1.6828500000000001E-3</v>
@@ -85672,7 +85676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">

</xml_diff>